<commit_message>
Burning changes and added field in office of profit
</commit_message>
<xml_diff>
--- a/phpdocx/template/MasterExcelFile.xlsx
+++ b/phpdocx/template/MasterExcelFile.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -221,17 +221,37 @@
   <si>
     <t>Company</t>
   </si>
+  <si>
+    <t>CSR</t>
+  </si>
+  <si>
+    <t>CSR as % of Net Profit</t>
+  </si>
+  <si>
+    <t>Jun'10</t>
+  </si>
+  <si>
+    <t>Jun'11</t>
+  </si>
+  <si>
+    <t>Jun'12</t>
+  </si>
+  <si>
+    <t>Jun'13</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="172" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -627,7 +647,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
@@ -635,8 +655,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -750,11 +771,21 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Comma 2" xfId="5"/>
     <cellStyle name="Comma 3" xfId="6"/>
+    <cellStyle name="Comma 4" xfId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Note" xfId="4" builtinId="10"/>
@@ -954,11 +985,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF000000"/>
+      <color rgb="FF464646"/>
       <color rgb="FFFFD200"/>
       <color rgb="FFD9D9D9"/>
-      <color rgb="FF464646"/>
       <color rgb="FF0000FF"/>
-      <color rgb="FF000000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1371,11 +1402,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="296111800"/>
-        <c:axId val="296113760"/>
+        <c:axId val="286240608"/>
+        <c:axId val="287058936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="296111800"/>
+        <c:axId val="286240608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1385,7 +1416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296113760"/>
+        <c:crossAx val="287058936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1393,7 +1424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296113760"/>
+        <c:axId val="287058936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1404,7 +1435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296111800"/>
+        <c:crossAx val="286240608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1542,6 +1573,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1606,6 +1638,123 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Audit Related Fee</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$96:$E$96</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY 12/13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY 13/14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY 14/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$98:$E$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5900000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12039999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$99</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Non Audit Fee </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1656,6 +1805,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1693,122 +1843,6 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$98:$E$98</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>4.5900000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.5999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.12039999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$99</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Non Audit Fee </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="65000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$96:$E$96</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>FY 12/13</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>FY 13/14</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>FY 14/15</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Sheet1!$C$99:$E$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1836,11 +1870,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="297211440"/>
-        <c:axId val="297210264"/>
+        <c:axId val="288002184"/>
+        <c:axId val="288002968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="297211440"/>
+        <c:axId val="288002184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,7 +1914,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297210264"/>
+        <c:crossAx val="288002968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1888,7 +1922,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297210264"/>
+        <c:axId val="288002968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +2033,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297211440"/>
+        <c:crossAx val="288002184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.000000000000001E-2"/>
@@ -2197,8 +2231,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="297213400"/>
-        <c:axId val="297216536"/>
+        <c:axId val="288004928"/>
+        <c:axId val="289435864"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2359,11 +2393,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="297216928"/>
-        <c:axId val="297214576"/>
+        <c:axId val="289437432"/>
+        <c:axId val="289431552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297213400"/>
+        <c:axId val="288004928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,7 +2425,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297216536"/>
+        <c:crossAx val="289435864"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2399,7 +2433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297216536"/>
+        <c:axId val="289435864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2464,12 +2498,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297213400"/>
+        <c:crossAx val="288004928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297214576"/>
+        <c:axId val="289431552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2479,12 +2513,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297216928"/>
+        <c:crossAx val="289437432"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="297216928"/>
+        <c:axId val="289437432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2494,7 +2528,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297214576"/>
+        <c:crossAx val="289431552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2671,6 +2705,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2720,11 +2755,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="297213792"/>
-        <c:axId val="297215360"/>
+        <c:axId val="289432728"/>
+        <c:axId val="289438608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="297213792"/>
+        <c:axId val="289432728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2744,7 +2779,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297215360"/>
+        <c:crossAx val="289438608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2752,7 +2787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297215360"/>
+        <c:axId val="289438608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2772,7 +2807,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297213792"/>
+        <c:crossAx val="289432728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2890,6 +2925,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2951,11 +2987,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="297209872"/>
-        <c:axId val="297217320"/>
+        <c:axId val="289437040"/>
+        <c:axId val="289433120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="297209872"/>
+        <c:axId val="289437040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2975,7 +3011,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297217320"/>
+        <c:crossAx val="289433120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2983,7 +3019,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297217320"/>
+        <c:axId val="289433120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3003,7 +3039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297209872"/>
+        <c:crossAx val="289437040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3336,11 +3372,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="297210656"/>
-        <c:axId val="297211832"/>
+        <c:axId val="289437824"/>
+        <c:axId val="289433904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="297210656"/>
+        <c:axId val="289437824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3360,7 +3396,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297211832"/>
+        <c:crossAx val="289433904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3368,7 +3404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297211832"/>
+        <c:axId val="289433904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3388,7 +3424,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297210656"/>
+        <c:crossAx val="289437824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3633,7 +3669,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3737,11 +3773,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="297213008"/>
-        <c:axId val="297212224"/>
+        <c:axId val="289438216"/>
+        <c:axId val="289436256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="297213008"/>
+        <c:axId val="289438216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3781,7 +3817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297212224"/>
+        <c:crossAx val="289436256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3789,7 +3825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297212224"/>
+        <c:axId val="289436256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3828,7 +3864,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297213008"/>
+        <c:crossAx val="289438216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3913,6 +3949,912 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13708910976291899"/>
+          <c:y val="0.17478642092815322"/>
+          <c:w val="0.85133565621370588"/>
+          <c:h val="0.58648611231288406"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="85000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="EB641B"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$493:$C$496</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jun'10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jun'11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jun'12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Jun'13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$493:$D$496</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.27529999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35349999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42509999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="332114936"/>
+        <c:axId val="332118856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="332114936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="332118856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="332118856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="332114936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln w="3175">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId2"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13708910976291899"/>
+          <c:y val="0.17478642092815322"/>
+          <c:w val="0.85133565621370588"/>
+          <c:h val="0.58648611231288406"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="85000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="EB641B"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$504:$C$507</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jun'10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jun'11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jun'12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Jun'13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$504:$D$507</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.27529999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35349999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42509999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="411204608"/>
+        <c:axId val="288553112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="411204608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="288553112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="288553112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411204608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln w="3175">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId2"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1401978782921591"/>
+          <c:y val="6.7712909339716562E-2"/>
+          <c:w val="0.67105686789151364"/>
+          <c:h val="0.64664125129155237"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$515</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CSR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="EB641B"/>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.4401821803252382E-3"/>
+                  <c:y val="2.4112661188156127E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$516:$C$518</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY 12/13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY 13/14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY 14/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$516:$D$518</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="411203432"/>
+        <c:axId val="411196376"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$515</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CSR as % of Net Profit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$516:$C$518</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY 12/13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY 13/14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY 14/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$516:$E$518</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="411203824"/>
+        <c:axId val="411200688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="411203432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411196376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="411196376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900"/>
+                  <a:t>CSR Contributions (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900">
+                    <a:latin typeface="Rupee Foradian"/>
+                  </a:rPr>
+                  <a:t>` </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900">
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Crore)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411203432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="411200688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900"/>
+                  <a:t>CSR as %</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900" baseline="0"/>
+                  <a:t> of net profit</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="900"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411203824"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="411203824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="411200688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.6718495631084089E-3"/>
+          <c:y val="0.80054773696274395"/>
+          <c:w val="0.99732811585515846"/>
+          <c:h val="0.13943349841450822"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId2"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
@@ -3934,9 +4876,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="1.1851851851851851E-2"/>
+          <c:x val="0.20919817190683335"/>
           <c:y val="2.9962546816479401E-2"/>
-          <c:w val="0.98222222222222222"/>
+          <c:w val="0.79080182809316668"/>
           <c:h val="0.64584926884139471"/>
         </c:manualLayout>
       </c:layout>
@@ -4007,6 +4949,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4120,6 +5063,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4178,11 +5122,11 @@
         </c:dLbls>
         <c:gapWidth val="90"/>
         <c:overlap val="-27"/>
-        <c:axId val="296113368"/>
-        <c:axId val="296111016"/>
+        <c:axId val="287533808"/>
+        <c:axId val="288333672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="296113368"/>
+        <c:axId val="287533808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4194,12 +5138,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:srgbClr val="464646"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -4222,7 +5163,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296111016"/>
+        <c:crossAx val="288333672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4230,17 +5171,106 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296111016"/>
+        <c:axId val="288333672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="&quot;₹&quot;\ #,##0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>In  Crores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296113368"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="287533808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4404,7 +5434,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4423,7 +5455,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4442,7 +5476,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4461,7 +5497,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="&quot;₹&quot;\ #,##0.00" sourceLinked="0"/>
@@ -4491,6 +5529,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4555,8 +5594,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="296112976"/>
-        <c:axId val="296110624"/>
+        <c:axId val="288333280"/>
+        <c:axId val="288334456"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4613,7 +5652,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4632,7 +5673,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4664,6 +5707,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4725,11 +5769,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="296114152"/>
-        <c:axId val="296112192"/>
+        <c:axId val="288332888"/>
+        <c:axId val="288331320"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="296110624"/>
+        <c:axId val="288334456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4780,12 +5824,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296112976"/>
+        <c:crossAx val="288333280"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="296112976"/>
+        <c:axId val="288333280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4805,7 +5849,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296110624"/>
+        <c:crossAx val="288334456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4813,7 +5857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296112192"/>
+        <c:axId val="288331320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4864,12 +5908,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296114152"/>
+        <c:crossAx val="288332888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="296114152"/>
+        <c:axId val="288332888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4879,7 +5923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296112192"/>
+        <c:crossAx val="288331320"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5018,7 +6062,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -5052,6 +6098,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -5148,6 +6195,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -5198,8 +6246,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="296400328"/>
-        <c:axId val="296399544"/>
+        <c:axId val="288331712"/>
+        <c:axId val="288332104"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5262,7 +6310,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5281,7 +6331,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5300,7 +6352,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="0.00%" sourceLinked="0"/>
@@ -5383,11 +6437,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="296404248"/>
-        <c:axId val="296400720"/>
+        <c:axId val="288004536"/>
+        <c:axId val="288332496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296400328"/>
+        <c:axId val="288331712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5407,7 +6461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296399544"/>
+        <c:crossAx val="288332104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5415,7 +6469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296399544"/>
+        <c:axId val="288332104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5437,6 +6491,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -5453,12 +6508,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296400328"/>
+        <c:crossAx val="288331712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="296400720"/>
+        <c:axId val="288332496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5505,12 +6560,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296404248"/>
+        <c:crossAx val="288004536"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="296404248"/>
+        <c:axId val="288004536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5520,7 +6575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="296400720"/>
+        <c:crossAx val="288332496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5687,7 +6742,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5807,11 +6864,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="296401112"/>
-        <c:axId val="296401896"/>
+        <c:axId val="288002576"/>
+        <c:axId val="288001008"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="296401112"/>
+        <c:axId val="288002576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5849,6 +6906,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5865,12 +6923,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296401896"/>
+        <c:crossAx val="288001008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="296401896"/>
+        <c:axId val="288001008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5908,6 +6966,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5924,7 +6983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296401112"/>
+        <c:crossAx val="288002576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6022,7 +7081,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6051,6 +7112,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -6146,6 +7208,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -6222,7 +7285,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6240,7 +7305,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6258,7 +7325,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6336,11 +7405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="296398760"/>
-        <c:axId val="296404640"/>
+        <c:axId val="288000224"/>
+        <c:axId val="288007280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="296398760"/>
+        <c:axId val="288000224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6360,7 +7429,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296404640"/>
+        <c:crossAx val="288007280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6368,7 +7437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296404640"/>
+        <c:axId val="288007280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6378,7 +7447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="296398760"/>
+        <c:crossAx val="288000224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8412,11 +9481,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296402680"/>
-        <c:axId val="296403464"/>
+        <c:axId val="288006496"/>
+        <c:axId val="287999832"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="296402680"/>
+        <c:axId val="288006496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="41449"/>
@@ -8438,7 +9507,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296403464"/>
+        <c:crossAx val="287999832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -8447,7 +9516,7 @@
         <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="296403464"/>
+        <c:axId val="287999832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="300"/>
@@ -8482,7 +9551,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296402680"/>
+        <c:crossAx val="288006496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8624,6 +9693,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -8705,6 +9775,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -8776,7 +9847,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -8810,6 +9883,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -8854,11 +9928,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="296397192"/>
-        <c:axId val="296403856"/>
+        <c:axId val="288005320"/>
+        <c:axId val="288004144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="296397192"/>
+        <c:axId val="288005320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8878,7 +9952,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296403856"/>
+        <c:crossAx val="288004144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8886,7 +9960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296403856"/>
+        <c:axId val="288004144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8906,7 +9980,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296397192"/>
+        <c:crossAx val="288005320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -8960,9 +10034,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0"/>
-          <c:y val="0.79741168540702845"/>
-          <c:w val="0.85419247237679807"/>
-          <c:h val="0.16731640062501912"/>
+          <c:y val="0.80778782029678198"/>
+          <c:w val="1"/>
+          <c:h val="0.10505959128649774"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -9117,7 +10191,9 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9285,7 +10361,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11547,6 +12625,96 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>490</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>532765</xdr:colOff>
+      <xdr:row>499</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="19" name="Chart 18"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>501</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>570865</xdr:colOff>
+      <xdr:row>511</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="21" name="Chart 20"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>513</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>525</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="22" name="Object 45"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12472,6 +13640,372 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00697</cdr:x>
+      <cdr:y>0.89011</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Text Box 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="20249" y="1543050"/>
+          <a:ext cx="2884876" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="900"/>
+            <a:t>Graph</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="900" baseline="0"/>
+            <a:t> xx: FII Shareholding in the Company</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="900"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.12637</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rectangle 1"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="2787015" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="1"/>
+            <a:t>FII Shareholdiing</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00697</cdr:x>
+      <cdr:y>0.89011</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Text Box 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="20249" y="1543050"/>
+          <a:ext cx="2884876" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="900"/>
+            <a:t>Graph</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="900" baseline="0"/>
+            <a:t> xx: FII Shareholding in the Company</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="900"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.12637</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rectangle 1"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="2787015" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="1"/>
+            <a:t>Promoter Shareholdiing</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.91075</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.91125</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Text Box 19"/>
+        <cdr:cNvSpPr txBox="1">
+          <a:spLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeArrowheads="1"/>
+        </cdr:cNvSpPr>
+      </cdr:nvSpPr>
+      <cdr:spPr bwMode="auto">
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="2219324"/>
+          <a:ext cx="3305175" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+        <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" anchorCtr="0" upright="1">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="900"/>
+            <a:t>Graph1: Peer comparison of Price/ Earnings ratio</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.89857</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.97396</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="Text Box 20"/>
+        <cdr:cNvSpPr txBox="1">
+          <a:spLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeArrowheads="1"/>
+        </cdr:cNvSpPr>
+      </cdr:nvSpPr>
+      <cdr:spPr bwMode="auto">
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="1643302"/>
+          <a:ext cx="2581275" cy="137873"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+        <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" anchorCtr="0" upright="1">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900">
+              <a:effectLst/>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Graph xx: CSR Contributions vs</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> Net Profits</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="900"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
@@ -12616,7 +14150,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-IN" sz="900" baseline="0"/>
-            <a:t> Average director remuneratiion</a:t>
+            <a:t> Average Director Remuneration</a:t>
           </a:r>
           <a:endParaRPr lang="en-IN" sz="900"/>
         </a:p>
@@ -14142,6 +15676,448 @@
       <a:font script="Viet" typeface="Arial"/>
       <a:font script="Uigh" typeface="Microsoft Uighur"/>
       <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:shade val="51000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="80000">
+            <a:schemeClr val="phClr">
+              <a:shade val="93000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="94000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride10.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Custom 2">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="464646"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="DEF5FA"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="2DA2BF"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="DA1F28"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="EB641B"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="464646"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="FFD200"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="002060"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="FF8119"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="44B9E8"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Custom 2">
+    <a:majorFont>
+      <a:latin typeface="Century Gothic"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:shade val="51000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="80000">
+            <a:schemeClr val="phClr">
+              <a:shade val="93000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="94000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride11.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Custom 2">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="464646"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="DEF5FA"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="2DA2BF"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="DA1F28"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="EB641B"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="464646"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="FFD200"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="002060"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="FF8119"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="44B9E8"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Custom 2">
+    <a:majorFont>
+      <a:latin typeface="Century Gothic"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
     </a:minorFont>
   </a:fontScheme>
   <a:fmtScheme name="Office">
@@ -15920,16 +17896,235 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride9.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Custom 2">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="464646"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="DEF5FA"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="2DA2BF"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="DA1F28"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="EB641B"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="464646"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="FFD200"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="002060"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="FF8119"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="44B9E8"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Custom 2">
+    <a:majorFont>
+      <a:latin typeface="Century Gothic"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:shade val="51000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="80000">
+            <a:schemeClr val="phClr">
+              <a:shade val="93000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="94000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B3:S485"/>
+  <dimension ref="B3:S518"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -19392,6 +21587,128 @@
         <v>50000</v>
       </c>
     </row>
+    <row r="492" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C492" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D492" s="61"/>
+    </row>
+    <row r="493" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C493" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="D493" s="63">
+        <v>0.27529999999999999</v>
+      </c>
+    </row>
+    <row r="494" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C494" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="D494" s="63">
+        <v>0.35139999999999999</v>
+      </c>
+    </row>
+    <row r="495" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C495" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="D495" s="63">
+        <v>0.35349999999999998</v>
+      </c>
+    </row>
+    <row r="496" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C496" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="D496" s="63">
+        <v>0.42509999999999998</v>
+      </c>
+    </row>
+    <row r="504" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C504" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="D504" s="65">
+        <v>0.27529999999999999</v>
+      </c>
+    </row>
+    <row r="505" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C505" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="D505" s="65">
+        <v>0.35139999999999999</v>
+      </c>
+    </row>
+    <row r="506" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C506" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="D506" s="65">
+        <v>0.35349999999999998</v>
+      </c>
+    </row>
+    <row r="507" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C507" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="D507" s="65">
+        <v>0.42509999999999998</v>
+      </c>
+    </row>
+    <row r="515" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C515" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="D515" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="E515" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="F515" s="66"/>
+      <c r="G515" s="66"/>
+    </row>
+    <row r="516" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C516" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="D516" s="69">
+        <v>4</v>
+      </c>
+      <c r="E516" s="68">
+        <v>0.4</v>
+      </c>
+      <c r="F516" s="66"/>
+      <c r="G516" s="66"/>
+    </row>
+    <row r="517" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C517" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="D517" s="69">
+        <v>4</v>
+      </c>
+      <c r="E517" s="68">
+        <v>0.4</v>
+      </c>
+      <c r="F517" s="66"/>
+      <c r="G517" s="66"/>
+    </row>
+    <row r="518" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C518" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="D518" s="69">
+        <v>2</v>
+      </c>
+      <c r="E518" s="68">
+        <v>0.2</v>
+      </c>
+      <c r="F518" s="66"/>
+      <c r="G518" s="66"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Burnining Issues and Director appointment issues fixed
</commit_message>
<xml_diff>
--- a/phpdocx/template/MasterExcelFile.xlsx
+++ b/phpdocx/template/MasterExcelFile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Jun'13</t>
+  </si>
+  <si>
+    <t>Indexed Profit</t>
   </si>
 </sst>
 </file>
@@ -1397,11 +1400,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="136426424"/>
-        <c:axId val="136427600"/>
+        <c:axId val="594767880"/>
+        <c:axId val="594768664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="136426424"/>
+        <c:axId val="594767880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136427600"/>
+        <c:crossAx val="594768664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1419,7 +1422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136427600"/>
+        <c:axId val="594768664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1430,7 +1433,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136426424"/>
+        <c:crossAx val="594767880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1568,6 +1571,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1684,6 +1688,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1798,6 +1803,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1862,11 +1868,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="322285336"/>
-        <c:axId val="322292392"/>
+        <c:axId val="361709216"/>
+        <c:axId val="361712744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="322285336"/>
+        <c:axId val="361709216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1906,7 +1912,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322292392"/>
+        <c:crossAx val="361712744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1914,7 +1920,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322292392"/>
+        <c:axId val="361712744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2025,7 +2031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322285336"/>
+        <c:crossAx val="361709216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.000000000000001E-2"/>
@@ -2223,8 +2229,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="322289648"/>
-        <c:axId val="322286512"/>
+        <c:axId val="361705688"/>
+        <c:axId val="361710000"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2283,19 +2289,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>111.3821138211382</c:v>
+                  <c:v>123.57723577235772</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>116.26016260162602</c:v>
+                  <c:v>119.51219512195121</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>122.76422764227641</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>119.51219512195121</c:v>
+                  <c:v>116.26016260162602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>123.57723577235772</c:v>
+                  <c:v>111.3821138211382</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2311,7 +2317,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Net Profit</c:v>
+                  <c:v>Indexed Profit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2356,19 +2362,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.205080756887725</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58.74010519681994</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.534878122122052</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.096908110525554</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2385,11 +2391,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="322290432"/>
-        <c:axId val="322286904"/>
+        <c:axId val="361711568"/>
+        <c:axId val="361706080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="322289648"/>
+        <c:axId val="361705688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2417,7 +2423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322286512"/>
+        <c:crossAx val="361710000"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2425,7 +2431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322286512"/>
+        <c:axId val="361710000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2490,12 +2496,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322289648"/>
+        <c:crossAx val="361705688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="322286904"/>
+        <c:axId val="361706080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,12 +2511,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="322290432"/>
+        <c:crossAx val="361711568"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="322290432"/>
+        <c:axId val="361711568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2520,7 +2526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="322286904"/>
+        <c:crossAx val="361706080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2697,6 +2703,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2746,11 +2753,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="322287296"/>
-        <c:axId val="322290040"/>
+        <c:axId val="361706472"/>
+        <c:axId val="361706864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="322287296"/>
+        <c:axId val="361706472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2770,7 +2777,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322290040"/>
+        <c:crossAx val="361706864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2778,7 +2785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322290040"/>
+        <c:axId val="361706864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +2805,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322287296"/>
+        <c:crossAx val="361706472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2916,6 +2923,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2977,11 +2985,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="322288080"/>
-        <c:axId val="322288472"/>
+        <c:axId val="121344704"/>
+        <c:axId val="121343136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="322288080"/>
+        <c:axId val="121344704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3001,7 +3009,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322288472"/>
+        <c:crossAx val="121343136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3009,7 +3017,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322288472"/>
+        <c:axId val="121343136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3029,7 +3037,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322288080"/>
+        <c:crossAx val="121344704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3311,7 +3319,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -3362,11 +3369,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="322819960"/>
-        <c:axId val="322823880"/>
+        <c:axId val="121342352"/>
+        <c:axId val="121345488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="322819960"/>
+        <c:axId val="121342352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3386,7 +3393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322823880"/>
+        <c:crossAx val="121345488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3394,7 +3401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322823880"/>
+        <c:axId val="121345488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3414,7 +3421,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322819960"/>
+        <c:crossAx val="121342352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3594,7 +3601,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3704,7 +3710,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3763,11 +3768,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="322818392"/>
-        <c:axId val="322821136"/>
+        <c:axId val="121345096"/>
+        <c:axId val="121340784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="322818392"/>
+        <c:axId val="121345096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3807,7 +3812,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322821136"/>
+        <c:crossAx val="121340784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3815,7 +3820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322821136"/>
+        <c:axId val="121340784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3854,7 +3859,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322818392"/>
+        <c:crossAx val="121345096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4044,6 +4049,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4099,11 +4105,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="322823096"/>
-        <c:axId val="322823488"/>
+        <c:axId val="121344312"/>
+        <c:axId val="121345880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="322823096"/>
+        <c:axId val="121344312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4123,7 +4129,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322823488"/>
+        <c:crossAx val="121345880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4131,7 +4137,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322823488"/>
+        <c:axId val="121345880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4151,7 +4157,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322823096"/>
+        <c:crossAx val="121344312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4279,6 +4285,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4334,11 +4341,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="322817608"/>
-        <c:axId val="322818000"/>
+        <c:axId val="121346272"/>
+        <c:axId val="121340392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="322817608"/>
+        <c:axId val="121346272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4358,7 +4365,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322818000"/>
+        <c:crossAx val="121340392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4366,7 +4373,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322818000"/>
+        <c:axId val="121340392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4386,7 +4393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322817608"/>
+        <c:crossAx val="121346272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4482,7 +4489,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -4516,6 +4525,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4565,8 +4575,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="322821920"/>
-        <c:axId val="322819176"/>
+        <c:axId val="121339216"/>
+        <c:axId val="121339608"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4643,11 +4653,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="322822312"/>
-        <c:axId val="322819568"/>
+        <c:axId val="121342744"/>
+        <c:axId val="121341960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="322821920"/>
+        <c:axId val="121339216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4667,7 +4677,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322819176"/>
+        <c:crossAx val="121339608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4675,7 +4685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322819176"/>
+        <c:axId val="121339608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4709,6 +4719,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -4725,12 +4736,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322821920"/>
+        <c:crossAx val="121339216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="322819568"/>
+        <c:axId val="121341960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4757,6 +4768,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
@@ -4773,12 +4785,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322822312"/>
+        <c:crossAx val="121342744"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="322822312"/>
+        <c:axId val="121342744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4788,7 +4800,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="322819568"/>
+        <c:crossAx val="121341960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4825,6 +4837,545 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId2"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10634903037761877"/>
+          <c:y val="4.9490026830164825E-2"/>
+          <c:w val="0.76538810796734513"/>
+          <c:h val="0.69262232979848626"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$530</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ED Remuneration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="EB641B"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$P$531:$P$535</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>FY10/11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY11/12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY12/13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FY13/14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FY14/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$531:$Q$535</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="359869496"/>
+        <c:axId val="359870672"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$530</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indexed TSR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="464646"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$P$531:$P$535</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>FY10/11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY11/12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY12/13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FY13/14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FY14/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$531:$R$535</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>123.57723577235772</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>119.51219512195121</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>122.76422764227641</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116.26016260162602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>111.3821138211382</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$530</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indexed Profit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFD200"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$P$531:$P$535</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>FY10/11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY11/12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY12/13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FY13/14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FY14/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$531:$S$535</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="359874592"/>
+        <c:axId val="359872632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="359869496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="808080"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359870672"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="0"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="359870672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900"/>
+                  <a:t>ED Remuneration (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900">
+                    <a:latin typeface="Rupee Foradian"/>
+                  </a:rPr>
+                  <a:t>`</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900"/>
+                  <a:t> Crore)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0"/>
+              <c:y val="0.14476936810335991"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="808080"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359869496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="359872632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="359874592"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="359874592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="359872632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0"/>
+          <c:y val="0.7865500210911136"/>
+          <c:w val="1"/>
+          <c:h val="0.17996783605174352"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
@@ -5103,11 +5654,11 @@
         </c:dLbls>
         <c:gapWidth val="90"/>
         <c:overlap val="-27"/>
-        <c:axId val="136426032"/>
-        <c:axId val="321610192"/>
+        <c:axId val="364486200"/>
+        <c:axId val="364488552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="136426032"/>
+        <c:axId val="364486200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5144,7 +5695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321610192"/>
+        <c:crossAx val="364488552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5152,7 +5703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="321610192"/>
+        <c:axId val="364488552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5241,7 +5792,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136426032"/>
+        <c:crossAx val="364486200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5405,9 +5956,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5426,9 +5975,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5447,9 +5994,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5468,9 +6013,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="&quot;₹&quot;\ #,##0.00" sourceLinked="0"/>
@@ -5500,7 +6043,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -5565,8 +6107,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="321605488"/>
-        <c:axId val="321605096"/>
+        <c:axId val="364489336"/>
+        <c:axId val="364487376"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5623,9 +6165,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5644,9 +6184,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5678,7 +6216,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -5740,11 +6277,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="321610584"/>
-        <c:axId val="321606664"/>
+        <c:axId val="364492864"/>
+        <c:axId val="364492472"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="321605096"/>
+        <c:axId val="364487376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5795,12 +6332,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321605488"/>
+        <c:crossAx val="364489336"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="321605488"/>
+        <c:axId val="364489336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5820,7 +6357,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321605096"/>
+        <c:crossAx val="364487376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5828,7 +6365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="321606664"/>
+        <c:axId val="364492472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5879,12 +6416,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321610584"/>
+        <c:crossAx val="364492864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="321610584"/>
+        <c:axId val="364492864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5894,7 +6431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="321606664"/>
+        <c:crossAx val="364492472"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6213,8 +6750,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="321609800"/>
-        <c:axId val="321608232"/>
+        <c:axId val="364487768"/>
+        <c:axId val="364489728"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6398,11 +6935,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="321603920"/>
-        <c:axId val="321604312"/>
+        <c:axId val="364486592"/>
+        <c:axId val="364491688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="321609800"/>
+        <c:axId val="364487768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6422,7 +6959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321608232"/>
+        <c:crossAx val="364489728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6430,7 +6967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="321608232"/>
+        <c:axId val="364489728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6468,12 +7005,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321609800"/>
+        <c:crossAx val="364487768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="321604312"/>
+        <c:axId val="364491688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6520,12 +7057,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321603920"/>
+        <c:crossAx val="364486592"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="321603920"/>
+        <c:axId val="364486592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6535,7 +7072,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="321604312"/>
+        <c:crossAx val="364491688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6822,11 +7359,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="321603136"/>
-        <c:axId val="321606272"/>
+        <c:axId val="364486984"/>
+        <c:axId val="364492080"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="321603136"/>
+        <c:axId val="364486984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6880,12 +7417,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321606272"/>
+        <c:crossAx val="364492080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="321606272"/>
+        <c:axId val="364492080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6939,7 +7476,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321603136"/>
+        <c:crossAx val="364486984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7037,7 +7574,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7066,6 +7605,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -7161,6 +7701,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -7237,7 +7778,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7255,7 +7798,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7273,7 +7818,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7351,11 +7898,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="321607056"/>
-        <c:axId val="321607448"/>
+        <c:axId val="364485808"/>
+        <c:axId val="364490120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="321607056"/>
+        <c:axId val="364485808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7375,7 +7922,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321607448"/>
+        <c:crossAx val="364490120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7383,7 +7930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="321607448"/>
+        <c:axId val="364490120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7393,7 +7940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="321607056"/>
+        <c:crossAx val="364485808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9427,11 +9974,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="321603528"/>
-        <c:axId val="321604704"/>
+        <c:axId val="361711960"/>
+        <c:axId val="361712352"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="321603528"/>
+        <c:axId val="361711960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="41449"/>
@@ -9453,7 +10000,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321604704"/>
+        <c:crossAx val="361712352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -9462,7 +10009,7 @@
         <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="321604704"/>
+        <c:axId val="361712352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="300"/>
@@ -9497,7 +10044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321603528"/>
+        <c:crossAx val="361711960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9639,6 +10186,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -9720,6 +10268,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -9791,7 +10340,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9825,6 +10376,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -9869,11 +10421,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="322292784"/>
-        <c:axId val="322291608"/>
+        <c:axId val="361710392"/>
+        <c:axId val="361707256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="322292784"/>
+        <c:axId val="361710392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9893,7 +10445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322291608"/>
+        <c:crossAx val="361707256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9901,7 +10453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="322291608"/>
+        <c:axId val="361707256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9921,7 +10473,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="322292784"/>
+        <c:crossAx val="361710392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -12409,15 +12961,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>173990</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12647,6 +13199,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>528</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>540</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="24" name="Chart 23"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13936,6 +14520,56 @@
             <a:t> Net Profits</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="900"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00726</cdr:x>
+      <cdr:y>0.88893</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.99967</cdr:x>
+      <cdr:y>0.99677</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Text Box 20"/>
+        <cdr:cNvSpPr txBox="1">
+          <a:spLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeArrowheads="1"/>
+        </cdr:cNvSpPr>
+      </cdr:nvSpPr>
+      <cdr:spPr bwMode="auto">
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="25867" y="1777527"/>
+          <a:ext cx="3535942" cy="215630"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+        <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" vert="horz" wrap="square" lIns="0" tIns="45720" rIns="0" bIns="45720" anchor="t" anchorCtr="0" upright="1">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="900"/>
+            <a:t>Graph xx: Executive compensation vs. Total shareholders return</a:t>
+          </a:r>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -16226,6 +16860,287 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride12.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Custom 3">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="464646"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="DEF5FA"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="00B050"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="DA1F28"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="EB641B"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="39639D"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="FFD200"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="1E1458"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="FF8119"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="44B9E8"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Angsana New"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Cordia New"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:shade val="51000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="80000">
+            <a:schemeClr val="phClr">
+              <a:shade val="93000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="94000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
 <a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <a:clrScheme name="Custom 3">
@@ -18059,10 +18974,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B3:S518"/>
+  <dimension ref="B3:S540"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A527" workbookViewId="0">
+      <selection activeCell="A536" sqref="A536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18602,7 +19517,7 @@
         <v>51</v>
       </c>
       <c r="S109" s="27" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="2:19" x14ac:dyDescent="0.35">
@@ -18627,12 +19542,12 @@
         <v>6</v>
       </c>
       <c r="R110" s="27">
-        <f>D110</f>
-        <v>111.3821138211382</v>
+        <f>D114</f>
+        <v>123.57723577235772</v>
       </c>
       <c r="S110" s="27">
-        <f>100*(POWER((E114/$E$115),(1/1))-1)</f>
-        <v>100</v>
+        <f>E114/$E$115*100</f>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="2:19" x14ac:dyDescent="0.35">
@@ -18657,12 +19572,12 @@
         <v>5</v>
       </c>
       <c r="R111" s="27">
-        <f>D111</f>
-        <v>116.26016260162602</v>
+        <f>D113</f>
+        <v>119.51219512195121</v>
       </c>
       <c r="S111" s="27">
-        <f>100*(POWER((E113/$E$115),(1/2))-1)</f>
-        <v>73.205080756887725</v>
+        <f>E113/$E$115*100</f>
+        <v>300</v>
       </c>
     </row>
     <row r="112" spans="2:19" x14ac:dyDescent="0.35">
@@ -18691,8 +19606,8 @@
         <v>122.76422764227641</v>
       </c>
       <c r="S112" s="27">
-        <f>100*(POWER((E112/$E$115),(1/3))-1)</f>
-        <v>58.74010519681994</v>
+        <f>E112/$E$115*100</f>
+        <v>400</v>
       </c>
     </row>
     <row r="113" spans="2:19" x14ac:dyDescent="0.35">
@@ -18717,12 +19632,12 @@
         <v>3</v>
       </c>
       <c r="R113" s="27">
-        <f>D113</f>
-        <v>119.51219512195121</v>
+        <f>D111</f>
+        <v>116.26016260162602</v>
       </c>
       <c r="S113" s="27">
-        <f>100*(POWER((E111/$E$115),(1/4))-1)</f>
-        <v>49.534878122122052</v>
+        <f>E111/$E$115*100</f>
+        <v>500</v>
       </c>
     </row>
     <row r="114" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -18747,12 +19662,12 @@
         <v>2</v>
       </c>
       <c r="R114" s="27">
-        <f>D114</f>
-        <v>123.57723577235772</v>
+        <f>D110</f>
+        <v>111.3821138211382</v>
       </c>
       <c r="S114" s="27">
-        <f>100*(POWER((E110/$E$115),(1/5))-1)</f>
-        <v>43.096908110525554</v>
+        <f>E110/$E$115*100</f>
+        <v>600</v>
       </c>
     </row>
     <row r="115" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -18765,6 +19680,7 @@
         <v>1</v>
       </c>
     </row>
+    <row r="118" spans="2:19" s="66" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="122" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C122" s="48" t="s">
         <v>34</v>
@@ -21648,6 +22564,193 @@
       <c r="F518" s="66"/>
       <c r="G518" s="66"/>
     </row>
+    <row r="530" spans="2:19" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P530" s="27"/>
+      <c r="Q530" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="R530" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="S530" s="27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="531" spans="2:19" s="66" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B531" s="29"/>
+      <c r="C531" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D531" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E531" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="P531" s="27" t="str">
+        <f>B536</f>
+        <v>FY10/11</v>
+      </c>
+      <c r="Q531" s="27">
+        <f>C536</f>
+        <v>6</v>
+      </c>
+      <c r="R531" s="27">
+        <f>D536</f>
+        <v>123.57723577235772</v>
+      </c>
+      <c r="S531" s="27">
+        <f>E536/$E$537*100</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="532" spans="2:19" s="66" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B532" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C532" s="27">
+        <v>2</v>
+      </c>
+      <c r="D532" s="27">
+        <v>111.3821138211382</v>
+      </c>
+      <c r="E532" s="43">
+        <v>6</v>
+      </c>
+      <c r="P532" s="27" t="str">
+        <f>B535</f>
+        <v>FY11/12</v>
+      </c>
+      <c r="Q532" s="27">
+        <f>C535</f>
+        <v>5</v>
+      </c>
+      <c r="R532" s="27">
+        <f>D535</f>
+        <v>119.51219512195121</v>
+      </c>
+      <c r="S532" s="27">
+        <f>E535/$E$537*100</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="533" spans="2:19" s="66" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B533" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C533" s="27">
+        <v>3</v>
+      </c>
+      <c r="D533" s="27">
+        <v>116.26016260162602</v>
+      </c>
+      <c r="E533" s="43">
+        <v>5</v>
+      </c>
+      <c r="P533" s="27" t="str">
+        <f>B534</f>
+        <v>FY12/13</v>
+      </c>
+      <c r="Q533" s="27">
+        <f>C534</f>
+        <v>4</v>
+      </c>
+      <c r="R533" s="27">
+        <f>D534</f>
+        <v>122.76422764227641</v>
+      </c>
+      <c r="S533" s="27">
+        <f>E534/$E$537*100</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="534" spans="2:19" s="66" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B534" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C534" s="27">
+        <v>4</v>
+      </c>
+      <c r="D534" s="27">
+        <v>122.76422764227641</v>
+      </c>
+      <c r="E534" s="43">
+        <v>4</v>
+      </c>
+      <c r="P534" s="27" t="str">
+        <f>B533</f>
+        <v>FY13/14</v>
+      </c>
+      <c r="Q534" s="27">
+        <f>C533</f>
+        <v>3</v>
+      </c>
+      <c r="R534" s="27">
+        <f>D533</f>
+        <v>116.26016260162602</v>
+      </c>
+      <c r="S534" s="27">
+        <f>E533/$E$537*100</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="535" spans="2:19" s="66" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B535" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C535" s="27">
+        <v>5</v>
+      </c>
+      <c r="D535" s="27">
+        <v>119.51219512195121</v>
+      </c>
+      <c r="E535" s="43">
+        <v>3</v>
+      </c>
+      <c r="P535" s="27" t="str">
+        <f>B532</f>
+        <v>FY14/15</v>
+      </c>
+      <c r="Q535" s="27">
+        <f>C532</f>
+        <v>2</v>
+      </c>
+      <c r="R535" s="27">
+        <f>D532</f>
+        <v>111.3821138211382</v>
+      </c>
+      <c r="S535" s="27">
+        <f>E532/$E$537*100</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="536" spans="2:19" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B536" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C536" s="44">
+        <v>6</v>
+      </c>
+      <c r="D536" s="44">
+        <v>123.57723577235772</v>
+      </c>
+      <c r="E536" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="537" spans="2:19" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B537" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C537" s="44"/>
+      <c r="D537" s="44"/>
+      <c r="E537" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="538" spans="2:19" s="66" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="539" spans="2:19" s="66" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="540" spans="2:19" s="66" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>